<commit_message>
update dataset - applications for pilot
</commit_message>
<xml_diff>
--- a/ExperimentApplicationFilter.xlsx
+++ b/ExperimentApplicationFilter.xlsx
@@ -5,10 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
-    <sheet name="Non-trivial" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Permission" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Duplication" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Maintenance" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Java" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Suitable" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="66">
   <si>
     <t xml:space="preserve">permission</t>
   </si>
@@ -31,13 +35,19 @@
     <t xml:space="preserve">calendar</t>
   </si>
   <si>
-    <t xml:space="preserve">nextcloud</t>
+    <t xml:space="preserve">Gadgetbridge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bangle.js Gadgetbridge</t>
   </si>
   <si>
     <t xml:space="preserve">Content Provider Helper</t>
   </si>
   <si>
-    <t xml:space="preserve">DAVx⁵ </t>
+    <t xml:space="preserve">Nextcloud</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DAVx⁵</t>
   </si>
   <si>
     <t xml:space="preserve">Element - Secure Messenger</t>
@@ -76,6 +86,9 @@
     <t xml:space="preserve">SMS Backup+</t>
   </si>
   <si>
+    <t xml:space="preserve">Digitales Klassenzimmer</t>
+  </si>
+  <si>
     <t xml:space="preserve">JKU App</t>
   </si>
   <si>
@@ -85,19 +98,40 @@
     <t xml:space="preserve">InTheClear</t>
   </si>
   <si>
-    <t xml:space="preserve">Plees-tracker</t>
+    <t xml:space="preserve">plees-tracker</t>
   </si>
   <si>
     <t xml:space="preserve">Easer (beta)</t>
   </si>
   <si>
+    <t xml:space="preserve">AlwaysOn | Always On Display</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Easer</t>
+  </si>
+  <si>
     <t xml:space="preserve">DecSync CC</t>
   </si>
   <si>
+    <t xml:space="preserve">Calendar Trigger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VirtualXposed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MinCal Widget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DashClock Widget</t>
+  </si>
+  <si>
     <t xml:space="preserve">Persian Calendar</t>
   </si>
   <si>
-    <t xml:space="preserve">ICSx⁵ </t>
+    <t xml:space="preserve">Casio G-Shock Smart Sync</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ICSx⁵</t>
   </si>
   <si>
     <t xml:space="preserve">ShiftCal</t>
@@ -106,27 +140,54 @@
     <t xml:space="preserve">Calendar Import-Export</t>
   </si>
   <si>
+    <t xml:space="preserve">PolyCal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Etar - OpenSource Calendar</t>
   </si>
   <si>
+    <t xml:space="preserve">Todo Agenda</t>
+  </si>
+  <si>
     <t xml:space="preserve">Suntimes Calendars</t>
   </si>
   <si>
+    <t xml:space="preserve">Reservator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offline Calendar</t>
+  </si>
+  <si>
     <t xml:space="preserve">Congress Fahrplan</t>
   </si>
   <si>
+    <t xml:space="preserve">Todo Agenda for Android 4 – 7.0</t>
+  </si>
+  <si>
     <t xml:space="preserve">Calendar Notifications</t>
   </si>
   <si>
+    <t xml:space="preserve">Birthday Adapter</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Calendar Color</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tacere</t>
   </si>
   <si>
+    <t xml:space="preserve">Polite Droid</t>
+  </si>
+  <si>
     <t xml:space="preserve">CalDAV Sync Adapter</t>
   </si>
   <si>
     <t xml:space="preserve">Standalone Calendar</t>
   </si>
   <si>
+    <t xml:space="preserve">Anton Widget</t>
+  </si>
+  <si>
     <t xml:space="preserve">Diary</t>
   </si>
   <si>
@@ -142,24 +203,42 @@
     <t xml:space="preserve">Simpletask Nextcloud</t>
   </si>
   <si>
+    <t xml:space="preserve">Simpletask (WebDAV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simpletask </t>
+  </si>
+  <si>
     <t xml:space="preserve">SyncOrg</t>
   </si>
   <si>
     <t xml:space="preserve">SimpleDo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MobileOrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">last update</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Java Percentage</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="166" formatCode="0.00%"/>
   </numFmts>
   <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -180,12 +259,14 @@
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -230,17 +311,33 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -260,24 +357,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B40"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B19" activeCellId="0" sqref="B19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.64"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="73.91"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="22.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="61.13"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="2" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="2" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" s="4" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -285,7 +382,7 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
@@ -293,7 +390,7 @@
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
@@ -301,7 +398,7 @@
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
@@ -309,7 +406,7 @@
       <c r="A5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -317,7 +414,7 @@
       <c r="A6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -325,7 +422,7 @@
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -333,7 +430,7 @@
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -341,7 +438,7 @@
       <c r="A9" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -349,7 +446,7 @@
       <c r="A10" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
@@ -357,7 +454,7 @@
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -365,7 +462,7 @@
       <c r="A12" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -373,7 +470,7 @@
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -381,7 +478,7 @@
       <c r="A14" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>15</v>
       </c>
     </row>
@@ -389,7 +486,7 @@
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
     </row>
@@ -397,7 +494,7 @@
       <c r="A16" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -405,7 +502,7 @@
       <c r="A17" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -413,7 +510,7 @@
       <c r="A18" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="2" t="s">
         <v>19</v>
       </c>
     </row>
@@ -421,7 +518,7 @@
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="2" t="s">
         <v>20</v>
       </c>
     </row>
@@ -429,7 +526,7 @@
       <c r="A20" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -437,7 +534,7 @@
       <c r="A21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -445,7 +542,7 @@
       <c r="A22" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="2" t="s">
         <v>23</v>
       </c>
     </row>
@@ -453,7 +550,7 @@
       <c r="A23" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="2" t="s">
         <v>24</v>
       </c>
     </row>
@@ -461,7 +558,7 @@
       <c r="A24" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="2" t="s">
         <v>25</v>
       </c>
     </row>
@@ -469,7 +566,7 @@
       <c r="A25" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="2" t="s">
         <v>26</v>
       </c>
     </row>
@@ -477,7 +574,7 @@
       <c r="A26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="2" t="s">
         <v>27</v>
       </c>
     </row>
@@ -485,7 +582,7 @@
       <c r="A27" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="2" t="s">
         <v>28</v>
       </c>
     </row>
@@ -493,7 +590,7 @@
       <c r="A28" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -501,7 +598,7 @@
       <c r="A29" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="B29" s="2" t="s">
         <v>30</v>
       </c>
     </row>
@@ -509,7 +606,7 @@
       <c r="A30" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="2" t="s">
         <v>31</v>
       </c>
     </row>
@@ -517,7 +614,7 @@
       <c r="A31" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="2" t="s">
         <v>32</v>
       </c>
     </row>
@@ -525,7 +622,7 @@
       <c r="A32" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="2" t="s">
         <v>33</v>
       </c>
     </row>
@@ -533,7 +630,7 @@
       <c r="A33" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="2" t="s">
         <v>34</v>
       </c>
     </row>
@@ -541,7 +638,7 @@
       <c r="A34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="2" t="s">
         <v>35</v>
       </c>
     </row>
@@ -549,7 +646,7 @@
       <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -557,7 +654,7 @@
       <c r="A36" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="1" t="s">
+      <c r="B36" s="2" t="s">
         <v>37</v>
       </c>
     </row>
@@ -565,7 +662,7 @@
       <c r="A37" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="2" t="s">
         <v>38</v>
       </c>
     </row>
@@ -573,7 +670,7 @@
       <c r="A38" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B38" s="1" t="s">
+      <c r="B38" s="2" t="s">
         <v>39</v>
       </c>
     </row>
@@ -581,7 +678,7 @@
       <c r="A39" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>40</v>
       </c>
     </row>
@@ -589,8 +686,184 @@
       <c r="A40" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B53" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B55" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B62" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -602,4 +875,926 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="61.13"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="2" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="61.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="37.23"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="5" t="n">
+        <v>44854</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="5" t="n">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="5" t="n">
+        <v>44861</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="5" t="n">
+        <v>44860</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="n">
+        <v>44859</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="5" t="n">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="5" t="n">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="5" t="n">
+        <v>44822</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="5" t="n">
+        <v>44732</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="5" t="n">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="5" t="n">
+        <v>44843</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="5" t="n">
+        <v>44078</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="5" t="n">
+        <v>44825</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="5" t="n">
+        <v>44806</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" s="5" t="n">
+        <v>44644</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="5" t="n">
+        <v>44416</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="5" t="n">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="5" t="n">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="5" t="n">
+        <v>44788</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="5" t="n">
+        <v>44677</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>44563</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>44365</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>44162</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>44860</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>44851</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>44849</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>44833</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>44788</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>44684</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>44664</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>44659</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>44649</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>44518</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>44363</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>43913</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>44870</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>44862</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>44857</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>44851</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>44820</v>
+      </c>
+    </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="61.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="28.34"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="6" t="n">
+        <v>0.995</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="6" t="n">
+        <v>0.712</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="n">
+        <v>0.899</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="6" t="n">
+        <v>0.919</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="6" t="n">
+        <v>0.802</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="6" t="n">
+        <v>0.978</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="6" t="n">
+        <v>0.986</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="6" t="n">
+        <v>0.943</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="6" t="n">
+        <v>0.999</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="6" t="n">
+        <v>0.798</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17" s="6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048553" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048554" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048555" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048556" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048557" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048558" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:A1048576"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="17.35" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="48.62"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>